<commit_message>
generacion de algunos resultados
</commit_message>
<xml_diff>
--- a/Resultados/P_1.xlsx
+++ b/Resultados/P_1.xlsx
@@ -67,7 +67,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="true"/>
+    <col min="1" max="1" width="14.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -77,242 +77,242 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2.0277639436714461</v>
+        <v>2.0096818918040058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.11785661247595752</v>
+        <v>0.10419017175436893</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.074246227068133636</v>
+        <v>0.06073459429499839</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.11787174018081603</v>
+        <v>0.10419086645753386</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.47796599477737145</v>
+        <v>0.46471381381104365</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.47796672622382819</v>
+        <v>0.46471389022953691</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>-0.00014908095248688386</v>
+        <v>-0.013365773974080092</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-0.0001494469198023464</v>
+        <v>-0.013365738697902568</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.25321951835167839</v>
+        <v>0.23980343489296019</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.021436655668303325</v>
+        <v>0.008111571558382916</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>-0.0063123492973395983</v>
+        <v>-0.019554380766878279</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.021883601255816121</v>
+        <v>0.0084885583754966114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.099002614509572498</v>
+        <v>0.085742461613731419</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.099004614251506209</v>
+        <v>0.085742478840539899</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>-0.012081542718279503</v>
+        <v>-0.025265524575219321</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>-0.012083427615977834</v>
+        <v>-0.025265513780247363</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>-0.010575015437446832</v>
+        <v>-0.023781880370353222</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.040004446726049997</v>
+        <v>0.026734490545885517</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>-0.010568442237939107</v>
+        <v>-0.023781433025612253</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.039166966440008145</v>
+        <v>0.025784614172220267</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.014225376668561338</v>
+        <v>0.0010160412959051776</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.014228692985044604</v>
+        <v>0.0010160437866119018</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>-0.013444139607270457</v>
+        <v>-0.0266043839074874</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>-0.013447416700944478</v>
+        <v>-0.026604371092488845</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>-0.0018446166912183034</v>
+        <v>-0.01501101430663007</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>-0.011519673760024765</v>
+        <v>-0.024666573486693193</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>-0.011491213278542673</v>
+        <v>-0.024641097271382584</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>-0.011524834485014356</v>
+        <v>-0.02466923616441908</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>-0.0087710546421074474</v>
+        <v>-0.021941043027680091</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>-0.0087676363221747076</v>
+        <v>-0.021941040828049856</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>-0.010645955204329286</v>
+        <v>-0.02381837558615885</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>-0.010649265966514956</v>
+        <v>-0.023818384041146626</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>-0.0094090379233504572</v>
+        <v>-0.022560861058491109</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>-0.0094926457738313749</v>
+        <v>-0.02265233644541105</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>-0.0095367389745743564</v>
+        <v>-0.022691416489542315</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>-0.0095225566197173518</v>
+        <v>-0.022675637466859262</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>-0.012011494312420122</v>
+        <v>-0.025175271490418535</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>-0.012009717431574926</v>
+        <v>-0.02517524525397458</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>-0.010592573121207816</v>
+        <v>-0.023766056087734674</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>-0.010594091243225589</v>
+        <v>-0.023766077738608553</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>-0.014192197536140285</v>
+        <v>-0.027372902024398661</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>-0.014191229685288438</v>
+        <v>-0.027372902212269269</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>-0.013275915305345255</v>
+        <v>-0.0264601265519449</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>-0.013276758801707658</v>
+        <v>-0.026460129125311784</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>-0.0086424108315527187</v>
+        <v>-0.021872934979597754</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>-0.0086367795725117973</v>
+        <v>-0.021872845896268551</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>-0.0053803422411134103</v>
+        <v>-0.018632828500986312</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>-0.0053865225072514981</v>
+        <v>-0.018632893238897167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>